<commit_message>
update result 20201202 & update plan 20201203
</commit_message>
<xml_diff>
--- a/20201202.xlsx
+++ b/20201202.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6932BF62-9B67-49D5-8D97-887B3C2A9893}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19794BF4-4377-4C0C-89D8-74BD631DFF33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -198,10 +198,6 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>1.저번주에 못지킨 월수금 약속 지키기(운동, 금식, 술안먹기, 아침에 공부) 33.3%</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t>로컬패킷 보낼 때 파일 포인터 기억하도록 변경</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
@@ -218,19 +214,25 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
+    <t>I2C analog filter 제거 테스트</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">어둠 코딩 </t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">
-1. 로그 분할 (진행중)
- - 용량에 따라 분할(완)
- - DS1338의 시간이 00년 00월 00일 00시 00분 00초로 들어옴
-  -&gt; I2C에서 ERROR가 난다. 한번나면 계속남</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t>I2C analog filter 제거 테스트</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">어둠 코딩 </t>
+1. I2C busy flag 이슈 수정
+ - analog filter 제거
+  -&gt; aging test 하루 간 문제발생 하지않음 (며칠 더 테스트 후 추가로 에러가 발생하지 않으면 픽 
+      스)
+2. LAN configration 추가 (진행중)
+ - LAN으로 MAC, IP등 변경할 수 있도록 기능 추가</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.저번주에 못지킨 월수금 약속 지키기(운동, 금식, 술안먹기, 아침에 공부) 66.6%</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -404,7 +406,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -612,6 +614,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -918,7 +944,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -973,46 +999,49 @@
     <xf numFmtId="176" fontId="1" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="1" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1548,7 +1577,7 @@
   <dimension ref="B2:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1616,18 +1645,18 @@
         <v>41</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="5"/>
       <c r="I3" s="11" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" t="s">
@@ -1745,13 +1774,13 @@
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="26"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="9"/>
       <c r="F10" s="14"/>
       <c r="G10" s="16"/>
@@ -1760,13 +1789,13 @@
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="26"/>
+      <c r="C11" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="27"/>
       <c r="E11" s="9"/>
       <c r="F11" s="14"/>
       <c r="G11" s="16"/>
@@ -1775,13 +1804,13 @@
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="26"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="9"/>
       <c r="F12" s="14"/>
       <c r="G12" s="16"/>
@@ -1790,13 +1819,13 @@
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="2:15" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="26"/>
+      <c r="C13" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="27"/>
       <c r="E13" s="9"/>
       <c r="F13" s="14"/>
       <c r="G13" s="16"/>
@@ -1805,13 +1834,13 @@
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="26"/>
+      <c r="D14" s="27"/>
       <c r="E14" s="9"/>
       <c r="F14" s="14"/>
       <c r="G14" s="16"/>
@@ -1820,13 +1849,13 @@
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="26"/>
+      <c r="C15" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="27"/>
       <c r="E15" s="9"/>
       <c r="F15" s="14"/>
       <c r="G15" s="16"/>
@@ -1835,13 +1864,13 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="2:15" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="26"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="9"/>
       <c r="F16" s="14"/>
       <c r="G16" s="16"/>
@@ -1850,13 +1879,13 @@
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="2:10" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="26"/>
+      <c r="C17" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="27"/>
       <c r="E17" s="9"/>
       <c r="F17" s="14"/>
       <c r="G17" s="16"/>
@@ -1865,13 +1894,13 @@
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="26"/>
+      <c r="D18" s="27"/>
       <c r="E18" s="9"/>
       <c r="F18" s="14"/>
       <c r="G18" s="16"/>
@@ -1880,13 +1909,13 @@
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="2:10" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="26"/>
+      <c r="D19" s="27"/>
       <c r="E19" s="9"/>
       <c r="F19" s="14"/>
       <c r="G19" s="16"/>
@@ -1895,13 +1924,13 @@
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="31"/>
+      <c r="C20" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="32"/>
       <c r="E20" s="9"/>
       <c r="F20" s="14"/>
       <c r="G20" s="16"/>
@@ -1910,13 +1939,13 @@
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="26"/>
+      <c r="C21" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="27"/>
       <c r="E21" s="9"/>
       <c r="F21" s="14"/>
       <c r="G21" s="16"/>
@@ -1925,13 +1954,13 @@
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="26"/>
+      <c r="D22" s="27"/>
       <c r="E22" s="9"/>
       <c r="F22" s="14"/>
       <c r="G22" s="16"/>
@@ -1940,13 +1969,13 @@
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="31"/>
+      <c r="C23" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="32"/>
       <c r="E23" s="10"/>
       <c r="F23" s="14"/>
       <c r="G23" s="17"/>

</xml_diff>